<commit_message>
Removed the intermediate node setup
and some other smaller changes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/abs_import_sheet(valid_1).xlsx
+++ b/src/test/resources/excel/abs_import_sheet(valid_1).xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/work/eclipse-workspace/abs-excel-converter/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/work/eclipse-workspace/abs-excel-converter/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19760" tabRatio="500"/>
+    <workbookView xWindow="5280" yWindow="-22920" windowWidth="33600" windowHeight="19760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Import-ID</t>
   </si>
@@ -413,7 +413,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,9 +514,6 @@
       <c r="G7" t="s">
         <v>8</v>
       </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">

</xml_diff>

<commit_message>
Updated the valid basic sheet
Removed the dash in Objectstatus
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/abs_import_sheet(valid_1).xlsx
+++ b/src/test/resources/excel/abs_import_sheet(valid_1).xlsx
@@ -53,9 +53,6 @@
     <t>Status x</t>
   </si>
   <si>
-    <t>As-designed</t>
-  </si>
-  <si>
     <t>Bestaand</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>OB00454</t>
+  </si>
+  <si>
+    <t>As designed</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,16 +461,16 @@
         <v>821</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
@@ -478,19 +478,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D5">
         <v>821</v>
       </c>
       <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -503,16 +503,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="G7" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -537,10 +537,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>